<commit_message>
Changes commit vk channel
</commit_message>
<xml_diff>
--- a/VootKidsSprint2.xlsx
+++ b/VootKidsSprint2.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="11850" activeTab="2"/>
+    <workbookView activeTab="1" windowHeight="11850" windowWidth="19200"/>
   </bookViews>
   <sheets>
-    <sheet name="Watch_history" sheetId="1" r:id="rId1"/>
-    <sheet name="Master" sheetId="2" r:id="rId2"/>
-    <sheet name="Channel" sheetId="4" r:id="rId3"/>
-    <sheet name="Watch" sheetId="5" r:id="rId4"/>
-    <sheet name="kidscharacters" sheetId="6" r:id="rId5"/>
-    <sheet name="gettraymedialist" sheetId="7" r:id="rId6"/>
+    <sheet name="Watch_history" r:id="rId1" sheetId="1"/>
+    <sheet name="Master" r:id="rId2" sheetId="2"/>
+    <sheet name="Channel" r:id="rId3" sheetId="4"/>
+    <sheet name="Watch" r:id="rId4" sheetId="5"/>
+    <sheet name="kidscharacters" r:id="rId5" sheetId="6"/>
+    <sheet name="gettraymedialist" r:id="rId6" sheetId="7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="1">
   <si>
     <t>TestType</t>
   </si>
@@ -225,46 +225,221 @@
     <t>channelName,channelId,sbu,imgURL</t>
   </si>
   <si>
+    <t>{
+    "assets": {
+        "title": "Channels",
+        "totalItems": 15,
+        "items": [
+            {
+                "channelName": "Nickelodeon 1",
+                "channelId": 3,
+                "sbu": "NICK1",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849940_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Entertainment one",
+                "channelId": 12,
+                "sbu": "ETO",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524837915_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Green Gold",
+                "channelId": 13,
+                "sbu": "GRG",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Hit Entertainment",
+                "channelId": 16,
+                "sbu": "HITENT",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849601_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Hi5",
+                "channelId": 15,
+                "sbu": "HI5",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849625_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Millimages",
+                "channelId": 18,
+                "sbu": "MIL",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849648_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Karadi Tales",
+                "channelId": 17,
+                "sbu": "KAR",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849720_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            }
+        ]
+    },
+    "status": {
+        "code": 200,
+        "message": "OK"
+    }
+}</t>
+  </si>
+  <si>
     <t>When all valid parameters with different offset and limit values</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
+    <t>{
+    "assets": {
+        "title": "Channels",
+        "totalItems": 15,
+        "items": [
+            {
+                "channelName": "Entertainment one",
+                "channelId": 12,
+                "sbu": "ETO",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524837915_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Green Gold",
+                "channelId": 13,
+                "sbu": "GRG",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Hit Entertainment",
+                "channelId": 16,
+                "sbu": "HITENT",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849601_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Hi5",
+                "channelId": 15,
+                "sbu": "HI5",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849625_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Millimages",
+                "channelId": 18,
+                "sbu": "MIL",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849648_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Karadi Tales",
+                "channelId": 17,
+                "sbu": "KAR",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849720_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Yoboho",
+                "channelId": 28,
+                "sbu": "YOB",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849755_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            },
+            {
+                "channelName": "Strika Entertainment",
+                "channelId": 21,
+                "sbu": "STR",
+                "imgURL": "https://voot-kids-cms.s3.amazonaws.com/voot-kids/include/upload/voot-kids-images/channel-logos/channel_1524849779_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"
+            }
+        ]
+    },
+    "status": {
+        "code": 200,
+        "message": "OK"
+    }
+}</t>
+  </si>
+  <si>
     <t>When invalid limit is passed</t>
   </si>
   <si>
     <t>The limit must be at least 1.</t>
   </si>
   <si>
+    <t>{
+    "assets": null,
+    "status": {
+        "code": 400,
+        "message": "The limit must be at least 1."
+    }
+}</t>
+  </si>
+  <si>
     <t>When alphanumeric chaaracters are passed in limit</t>
   </si>
   <si>
     <t>limit parameter must be numeric</t>
   </si>
   <si>
+    <t>{
+    "assets": null,
+    "status": {
+        "code": 400,
+        "message": "limit parameter must be numeric"
+    }
+}</t>
+  </si>
+  <si>
     <t>When empty limit is passed</t>
   </si>
   <si>
     <t>The limit field is required.</t>
   </si>
   <si>
+    <t>{
+    "assets": null,
+    "status": {
+        "code": 400,
+        "message": "The limit field is required."
+    }
+}</t>
+  </si>
+  <si>
+    <t>{"assets":{"title":"Channels","totalItems":15,"items":[{"channelName":"Nickelodeon 1","channelId":3,"sbu":"NICK1","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849940_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Entertainment one","channelId":12,"sbu":"ETO","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524837915_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Green Gold","channelId":13,"sbu":"GRG","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Hit Entertainment","channelId":16,"sbu":"HITENT","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849601_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Hi5","channelId":15,"sbu":"HI5","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849625_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Millimages","channelId":18,"sbu":"MIL","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849648_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Karadi Tales","channelId":17,"sbu":"KAR","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849720_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Yoboho","channelId":28,"sbu":"YOB","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849755_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Strika Entertainment","channelId":21,"sbu":"STR","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849779_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Wide Angle Media","channelId":27,"sbu":"WAM","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849803_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"TURNER","channelId":24,"sbu":"TUR","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849830_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Hasbro","channelId":14,"sbu":"HBRP","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1523978839_2.jpg"},{"channelName":"Toonz Animation","channelId":23,"sbu":"TOON","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524849990_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"},{"channelName":"Dandelooo","channelId":10,"sbu":"DAN","imgURL":"http:\/\/voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1523881413_2.jpg"},{"channelName":"Dream Theatre","channelId":11,"sbu":"DTH","imgURL":"https://voot-kids-cms.s3.amazonaws.com\/voot-kids\/include\/upload\/voot-kids-images\/channel-logos\/channel_1524850238_channel_1524837985_channel_1524047975_channel_1523885606_2.jpg"}]},"status":{"code":200,"message":"OK"}}</t>
+  </si>
+  <si>
     <t>When invalid offSet is passed</t>
   </si>
   <si>
     <t>The offSet must be at least 0.</t>
   </si>
   <si>
+    <t>{
+    "assets": null,
+    "status": {
+        "code": 400,
+        "message": "The offSet must be at least 0."
+    }
+}</t>
+  </si>
+  <si>
     <t>When alphanumeric characters are passed in offSet</t>
   </si>
   <si>
     <t>offSet parameter must be numeric</t>
   </si>
   <si>
+    <t>{
+    "assets": null,
+    "status": {
+        "code": 400,
+        "message": "offSet parameter must be numeric"
+    }
+}</t>
+  </si>
+  <si>
     <t>When Special Characters are passed in offSet</t>
   </si>
   <si>
     <t>When empty offSet is passed</t>
+  </si>
+  <si>
+    <t>{
+    "assets": null,
+    "status": {
+        "code": 400,
+        "message": "offSet parameter is required"
+    }
+}</t>
   </si>
   <si>
     <t>When null value is passed in offSet</t>
@@ -607,15 +782,6 @@
     <t>when invalid limit is passed</t>
   </si>
   <si>
-    <t>{
-    "assets": null,
-    "status": {
-        "code": 400,
-        "message": "The limit must be at least 1."
-    }
-}</t>
-  </si>
-  <si>
     <t>when Alpha numeric is passed</t>
   </si>
   <si>
@@ -634,15 +800,6 @@
     <t>@</t>
   </si>
   <si>
-    <t>{
-    "assets": null,
-    "status": {
-        "code": 400,
-        "message": "The limit field is required."
-    }
-}</t>
-  </si>
-  <si>
     <t>When offset is Notpassed</t>
   </si>
   <si>
@@ -666,15 +823,6 @@
     "status": {
         "code": 400,
         "message": "offSet value must be numeric"
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "assets": null,
-    "status": {
-        "code": 400,
-        "message": "offSet parameter is required"
     }
 }</t>
   </si>
@@ -1139,33 +1287,6 @@
     <t>a1</t>
   </si>
   <si>
-    <t>{
-    "assets": null,
-    "status": {
-        "code": 400,
-        "message": "limit parameter must be numeric"
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "assets": null,
-    "status": {
-        "code": 400,
-        "message": "The offSet must be at least 0."
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "assets": null,
-    "status": {
-        "code": 400,
-        "message": "offSet parameter must be numeric"
-    }
-}</t>
-  </si>
-  <si>
     <t>moduleId</t>
   </si>
   <si>
@@ -1370,6 +1491,9 @@
     }
 }</t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
@@ -1377,9 +1501,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2045,291 +2169,291 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="177">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="176">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="179">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="178">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="13" fillId="5" fontId="12" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="0" fontId="13" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="18" fillId="17" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="14" fillId="0" fontId="22" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="16" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="19" fillId="21" fontId="24" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="26" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="17" fillId="16" fontId="21" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="19" fillId="16" fontId="27" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="20" fillId="0" fontId="25" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="15" fillId="0" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="23" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="18" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="39">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="10" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="10"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2343,10 +2467,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2510,21 +2634,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2541,7 +2665,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2594,9 +2718,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -2604,13 +2728,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="67.8571428571429" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="52.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="44" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85714285714286" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.4285714285714" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="67.8571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="52.1428571428571" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.1428571428571" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="9.85714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2905,7 +3029,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:8">
+    <row customFormat="1" r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -2931,7 +3055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:8">
+    <row customFormat="1" r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2957,7 +3081,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:8">
+    <row customFormat="1" r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -2983,7 +3107,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:8">
+    <row customFormat="1" r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -3009,7 +3133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" customFormat="1" spans="1:8">
+    <row customFormat="1" r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -3035,7 +3159,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" customFormat="1" spans="1:8">
+    <row customFormat="1" r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3061,7 +3185,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" customFormat="1" spans="1:8">
+    <row customFormat="1" r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -3087,7 +3211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" customFormat="1" spans="1:8">
+    <row customFormat="1" r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3115,42 +3239,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" tooltip="http://apiuat.vootkids.com/app/ks/v1/watchhistory.json"/>
-    <hyperlink ref="C4" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C5" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C6" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C7" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C8" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C9" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C10" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C11" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C12" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C13" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C14" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C15" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C3" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C16" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C17" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C18" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
-    <hyperlink ref="C19" r:id="rId1" display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C2" tooltip="http://apiuat.vootkids.com/app/ks/v1/watchhistory.json"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C4"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C5"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C6"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C7"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C8"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C9"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C10"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C11"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C12"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C13"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C14"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C15"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C3"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C16"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C17"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C18"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/ks/v1/watchHistory.json" r:id="rId1" ref="C19"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4" outlineLevelRow="5"/>
   <cols>
-    <col min="2" max="2" width="26.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="26.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3170,119 +3294,77 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:2">
       <c r="A2" s="30">
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>18</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="32">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="C3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="32">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="32">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="32">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3">
-      <c r="C7">
-        <f>SUM(C2:C6)</f>
-        <v>96</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="58.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="6" max="6" width="15.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="37" customWidth="1"/>
-    <col min="9" max="9" width="13.8571428571429" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="58.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="64.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.7142857142857" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.8571428571429" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3317,7 +3399,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -3339,19 +3421,25 @@
       <c r="G2" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>19</v>
@@ -3362,13 +3450,19 @@
       <c r="G3" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>65</v>
@@ -3383,15 +3477,21 @@
         <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>65</v>
@@ -3406,10 +3506,16 @@
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -3429,15 +3535,21 @@
         <v>16</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>65</v>
@@ -3452,10 +3564,16 @@
         <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -3475,10 +3593,16 @@
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -3500,13 +3624,19 @@
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>65</v>
@@ -3521,15 +3651,21 @@
         <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>83</v>
+      </c>
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>65</v>
@@ -3544,15 +3680,21 @@
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>86</v>
+      </c>
+      <c r="H11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>65</v>
@@ -3567,15 +3709,21 @@
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>86</v>
+      </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>65</v>
@@ -3592,13 +3740,19 @@
       <c r="G13" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>65</v>
@@ -3613,15 +3767,21 @@
         <v>16</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>65</v>
@@ -3638,33 +3798,39 @@
       <c r="G15" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" tooltip="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C3" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C4" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C6" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C5" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C7" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C8" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C9" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C10" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C11" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C12" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C13" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C14" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
-    <hyperlink ref="C15" r:id="rId1" display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C2" tooltip="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C3"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C4"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C6"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C5"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C7"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C8"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C9"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C10"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C11"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C12"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C13"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C14"/>
+    <hyperlink display="http://apiuat.vootkids.com/app/curated/v1/tvChannelList.json" r:id="rId1" ref="C15"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView topLeftCell="D26" workbookViewId="0">
       <selection activeCell="M31" sqref="M31"/>
@@ -3672,14 +3838,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="42.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.85714285714286" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="49.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="42.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.2857142857143" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.85714285714286" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.1428571428571" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.7142857142857" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.7142857142857" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3702,10 +3868,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -3720,30 +3886,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="34" customHeight="1" spans="1:12">
+    <row customHeight="1" ht="34" r="2" spans="1:12">
       <c r="A2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>16</v>
@@ -3752,13 +3918,13 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" ht="38" customHeight="1" spans="1:12">
+    <row customHeight="1" ht="38" r="3" spans="1:12">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -3766,22 +3932,22 @@
         <v>11</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>16</v>
@@ -3790,21 +3956,21 @@
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" ht="55" customHeight="1" spans="1:12">
+    <row customHeight="1" ht="55" r="4" spans="1:12">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D4" s="35" t="s">
         <v>37</v>
@@ -3813,36 +3979,36 @@
         <v>14</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" ht="58" customHeight="1" spans="1:12">
+    <row customHeight="1" ht="58" r="5" spans="1:12">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>40</v>
@@ -3851,13 +4017,13 @@
         <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>16</v>
@@ -3866,36 +4032,36 @@
         <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="L5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" ht="60" spans="1:12">
+    <row ht="60" r="6" spans="1:12">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
@@ -3904,21 +4070,21 @@
         <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="L6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" ht="60" spans="1:12">
+    <row ht="60" r="7" spans="1:12">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>32</v>
@@ -3927,28 +4093,28 @@
         <v>14</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" ht="60" spans="1:12">
+    <row ht="60" r="8" spans="1:12">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3956,7 +4122,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>30</v>
@@ -3965,13 +4131,13 @@
         <v>14</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
@@ -3980,36 +4146,36 @@
         <v>23</v>
       </c>
       <c r="K8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row ht="60" r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="35" t="s">
         <v>97</v>
-      </c>
-      <c r="L8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" ht="60" spans="1:12">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>88</v>
       </c>
       <c r="E9" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>16</v>
@@ -4018,21 +4184,21 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" ht="60.75" spans="1:12">
+    <row ht="60.75" r="10" spans="1:12">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
@@ -4041,13 +4207,13 @@
         <v>14</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>16</v>
@@ -4056,74 +4222,74 @@
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" ht="60.75" spans="1:12">
+    <row ht="60.75" r="11" spans="1:12">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="K11" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="L11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" ht="60.75" spans="1:12">
+    <row ht="60.75" r="12" spans="1:12">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>16</v>
@@ -4132,36 +4298,36 @@
         <v>41</v>
       </c>
       <c r="K12" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="L12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" ht="60.75" spans="1:12">
+    <row ht="60.75" r="13" spans="1:12">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="H13" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I13" s="22" t="s">
         <v>16</v>
@@ -4170,36 +4336,36 @@
         <v>41</v>
       </c>
       <c r="K13" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="L13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" ht="60.75" spans="1:12">
+    <row ht="60.75" r="14" spans="1:12">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I14" s="22" t="s">
         <v>16</v>
@@ -4208,36 +4374,36 @@
         <v>45</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="L14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" ht="60.75" spans="1:12">
+    <row ht="60.75" r="15" spans="1:12">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>16</v>
@@ -4246,36 +4412,36 @@
         <v>41</v>
       </c>
       <c r="K15" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="L15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" ht="60.75" spans="1:12">
+    <row ht="60.75" r="16" spans="1:12">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>16</v>
@@ -4284,188 +4450,188 @@
         <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" ht="75.75" spans="1:12">
+    <row ht="75.75" r="17" spans="1:12">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="K17" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" ht="60.75" spans="1:12">
+    <row ht="60.75" r="18" spans="1:12">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E18" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="K18" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="L18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" ht="60.75" spans="1:12">
+    <row ht="60.75" r="19" spans="1:12">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
         <v>30</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="K19" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="L19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" ht="60.75" spans="1:12">
+    <row ht="60.75" r="20" spans="1:12">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E20" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G20" t="s">
         <v>35</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="K20" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="L20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" ht="30.75" spans="1:12">
+    <row ht="30.75" r="21" spans="1:12">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E21" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>16</v>
@@ -4474,24 +4640,24 @@
         <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" ht="45.75" spans="1:12">
+    <row ht="45.75" r="22" spans="1:12">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>14</v>
@@ -4500,36 +4666,36 @@
         <v>32</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="K22" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="L22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" ht="45.75" spans="1:12">
+    <row ht="45.75" r="23" spans="1:12">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E23" s="35" t="s">
         <v>14</v>
@@ -4538,36 +4704,36 @@
         <v>30</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="K23" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="L23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" ht="45.75" spans="1:12">
+    <row ht="45.75" r="24" spans="1:12">
       <c r="A24" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E24" s="35" t="s">
         <v>14</v>
@@ -4576,48 +4742,48 @@
         <v>35</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="K24" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="L24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" ht="60.75" spans="1:12">
+    <row ht="60.75" r="25" spans="1:12">
       <c r="A25" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>16</v>
@@ -4626,71 +4792,71 @@
         <v>17</v>
       </c>
       <c r="K25" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" ht="75.75" spans="1:12">
+    <row ht="75.75" r="26" spans="1:12">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="K26" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="L26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" ht="60.75" spans="1:12">
+    <row ht="60.75" r="27" spans="1:12">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H27" t="s">
         <v>32</v>
@@ -4699,36 +4865,36 @@
         <v>16</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="K27" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="L27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" ht="60.75" spans="1:12">
+    <row ht="60.75" r="28" spans="1:12">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E28" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H28" t="s">
         <v>30</v>
@@ -4737,36 +4903,36 @@
         <v>16</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="K28" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="L28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" ht="60.75" spans="1:12">
+    <row ht="60.75" r="29" spans="1:12">
       <c r="A29" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E29" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H29" t="s">
         <v>35</v>
@@ -4775,27 +4941,27 @@
         <v>16</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="K29" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="L29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" ht="51" customHeight="1" spans="1:12">
+    <row customHeight="1" ht="51" r="30" spans="1:12">
       <c r="A30" t="s">
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E30" s="35" t="s">
         <v>14</v>
@@ -4813,24 +4979,24 @@
         <v>16</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="K30" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="L30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" ht="60" spans="1:12">
+    <row ht="60" r="31" spans="1:12">
       <c r="A31" t="s">
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
         <v>35</v>
@@ -4839,13 +5005,13 @@
         <v>35</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>16</v>
@@ -4854,22 +5020,22 @@
         <v>17</v>
       </c>
       <c r="K31" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="L31" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
@@ -4877,9 +5043,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="57.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="37.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="57.7142857142857" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4916,10 +5082,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>13</v>
@@ -4934,24 +5100,24 @@
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="I2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" ht="30" spans="1:9">
+    <row ht="30" r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>19</v>
@@ -4963,21 +5129,21 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="I3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" ht="30.75" spans="1:9">
+    <row ht="30.75" r="4" spans="1:9">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>37</v>
@@ -4989,27 +5155,27 @@
         <v>16</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" ht="30.75" spans="1:9">
+    <row ht="30.75" r="5" spans="1:9">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>14</v>
@@ -5018,16 +5184,16 @@
         <v>16</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" ht="30.75" spans="1:9">
+    <row ht="30.75" r="6" spans="1:9">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -5035,10 +5201,10 @@
         <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>14</v>
@@ -5047,24 +5213,24 @@
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" ht="30.75" spans="1:9">
+    <row ht="30.75" r="7" spans="1:9">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -5076,16 +5242,16 @@
         <v>16</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" ht="30.75" spans="1:9">
+    <row ht="30.75" r="8" spans="1:9">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -5093,7 +5259,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -5105,16 +5271,16 @@
         <v>16</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" ht="33" customHeight="1" spans="1:9">
+    <row customHeight="1" ht="33" r="9" spans="1:9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5122,7 +5288,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
@@ -5134,24 +5300,24 @@
         <v>16</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" ht="30.75" spans="1:9">
+    <row ht="30.75" r="10" spans="1:9">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>13</v>
@@ -5163,82 +5329,82 @@
         <v>16</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row ht="30.75" r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" ht="30.75" spans="1:9">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="D11" s="37" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="I11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" ht="30.75" spans="1:9">
+    <row ht="30.75" r="12" spans="1:9">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" ht="30.75" spans="1:9">
+    <row ht="30.75" r="13" spans="1:9">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>13</v>
@@ -5253,21 +5419,21 @@
         <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="I13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" ht="30.75" spans="1:9">
+    <row ht="30.75" r="14" spans="1:9">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>13</v>
@@ -5279,24 +5445,24 @@
         <v>16</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" ht="30.75" spans="1:9">
+    <row ht="30.75" r="15" spans="1:9">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D15" s="37" t="s">
         <v>13</v>
@@ -5311,22 +5477,22 @@
         <v>45</v>
       </c>
       <c r="H15" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="I15" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
@@ -5334,11 +5500,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="59.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7142857142857" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="56.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="41.5714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="59.7142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.7142857142857" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="56.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5352,7 +5518,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -5373,21 +5539,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:10">
+    <row ht="15.75" r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>14</v>
@@ -5399,27 +5565,27 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" ht="51" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="51" r="3" spans="1:10">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>19</v>
@@ -5431,27 +5597,27 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:10">
+    <row ht="15.75" r="4" spans="1:10">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>151</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>148</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>14</v>
@@ -5460,30 +5626,30 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" ht="32" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="32" r="5" spans="1:10">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>14</v>
@@ -5492,30 +5658,30 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I5" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" ht="30.75" spans="1:10">
+    <row ht="30.75" r="6" spans="1:10">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>14</v>
@@ -5524,30 +5690,30 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" ht="24" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="24" r="7" spans="1:10">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>14</v>
@@ -5556,30 +5722,30 @@
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" ht="24" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="24" r="8" spans="1:10">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>19</v>
@@ -5588,30 +5754,30 @@
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:10">
+    <row ht="15.75" r="9" spans="1:10">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>14</v>
@@ -5620,30 +5786,30 @@
         <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" ht="24" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="24" r="10" spans="1:10">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>14</v>
@@ -5652,27 +5818,27 @@
         <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" ht="30.75" spans="1:10">
+    <row ht="30.75" r="11" spans="1:10">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -5687,13 +5853,13 @@
         <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" ht="21" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="21" r="12" spans="1:10">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -5701,13 +5867,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F12" s="37" t="s">
         <v>14</v>
@@ -5719,24 +5885,24 @@
         <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:10">
+    <row ht="15.75" r="13" spans="1:10">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -5748,16 +5914,16 @@
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" ht="18" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="18" r="14" spans="1:10">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5765,10 +5931,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -5783,13 +5949,13 @@
         <v>23</v>
       </c>
       <c r="I14" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" ht="70" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="70" r="15" spans="1:10">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -5797,10 +5963,10 @@
         <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -5815,62 +5981,62 @@
         <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" ht="16" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="16" r="16" spans="1:10">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D16" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row ht="30.75" r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" t="s">
         <v>147</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" t="s">
-        <v>104</v>
-      </c>
-      <c r="J16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" ht="30.75" spans="1:10">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="F17" t="s">
-        <v>141</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
@@ -5879,30 +6045,30 @@
         <v>41</v>
       </c>
       <c r="I17" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="J17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" ht="22" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="22" r="18" spans="1:10">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F18" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
         <v>16</v>
@@ -5911,27 +6077,27 @@
         <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="J18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="1:10">
+    <row ht="15.75" r="19" spans="1:10">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F19" t="s">
         <v>32</v>
@@ -5943,27 +6109,27 @@
         <v>45</v>
       </c>
       <c r="I19" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="J19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" ht="24" customHeight="1" spans="1:10">
+    <row customHeight="1" ht="24" r="20" spans="1:10">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F20" t="s">
         <v>30</v>
@@ -5975,27 +6141,27 @@
         <v>41</v>
       </c>
       <c r="I20" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="J20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="1:10">
+    <row ht="15.75" r="21" spans="1:10">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F21" t="s">
         <v>35</v>
@@ -6007,14 +6173,14 @@
         <v>45</v>
       </c>
       <c r="I21" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="J21" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>